<commit_message>
completed domain and range
</commit_message>
<xml_diff>
--- a/UAS.xlsx
+++ b/UAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anishainasizdihar/Desktop/Battlefield/semantic/tugas3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7879AB92-3E54-9C45-943C-780D641318ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475E9AF4-DF87-D943-95A4-1D478C739C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22000" yWindow="0" windowWidth="11600" windowHeight="17440" xr2:uid="{E80C9FF6-146B-EE4D-BBAC-FC3E260E7FF3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <t>University</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>affiliatedTo</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>DateTime</t>
   </si>
 </sst>
 </file>
@@ -169,12 +175,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -189,8 +201,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6BB5E6-1A39-824F-9BFC-549AF7ACBA27}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,6 +640,11 @@
         <v>34</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>0</v>
@@ -703,6 +721,9 @@
       <c r="F29" t="s">
         <v>38</v>
       </c>
+      <c r="G29" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -723,7 +744,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -745,7 +766,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -783,5 +804,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed all requirements and restrictions
</commit_message>
<xml_diff>
--- a/UAS.xlsx
+++ b/UAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anishainasizdihar/Desktop/Battlefield/semantic/tugas3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475E9AF4-DF87-D943-95A4-1D478C739C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A136FB0C-04C7-7245-AE5F-06E1ECC00C7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22000" yWindow="0" windowWidth="11600" windowHeight="17440" xr2:uid="{E80C9FF6-146B-EE4D-BBAC-FC3E260E7FF3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>University</t>
   </si>
@@ -160,6 +160,30 @@
   </si>
   <si>
     <t>DateTime</t>
+  </si>
+  <si>
+    <t>publishYear</t>
+  </si>
+  <si>
+    <t>productionYear</t>
+  </si>
+  <si>
+    <t>numOfCopies</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>hasMentored</t>
+  </si>
+  <si>
+    <t>authorOf</t>
+  </si>
+  <si>
+    <t>directorOf</t>
+  </si>
+  <si>
+    <t>producerOf</t>
   </si>
 </sst>
 </file>
@@ -518,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6BB5E6-1A39-824F-9BFC-549AF7ACBA27}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,6 +759,15 @@
       <c r="C30" t="s">
         <v>14</v>
       </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -746,6 +779,15 @@
       <c r="C31" t="s">
         <v>16</v>
       </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -757,6 +799,15 @@
       <c r="C32" t="s">
         <v>31</v>
       </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -800,6 +851,50 @@
       </c>
       <c r="C36" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>